<commit_message>
Modified file --> add some details to charte de projet
</commit_message>
<xml_diff>
--- a/Reporting_indiv.xlsx
+++ b/Reporting_indiv.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="28">
   <si>
     <r>
       <rPr>
@@ -162,6 +162,9 @@
   </si>
   <si>
     <t>Evaluation des charges et calendrier cible</t>
+  </si>
+  <si>
+    <t>Julie</t>
   </si>
 </sst>
 </file>
@@ -1199,7 +1202,7 @@
   <dimension ref="B1:I23"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="26.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1357,76 +1360,136 @@
       <c r="B9" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="C9" s="14"/>
-      <c r="D9" s="14"/>
-      <c r="E9" s="15"/>
-      <c r="F9" s="15"/>
-      <c r="G9" s="18"/>
+      <c r="C9" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="D9" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="E9" s="15">
+        <v>42468</v>
+      </c>
+      <c r="F9" s="15">
+        <v>42472</v>
+      </c>
+      <c r="G9" s="16">
+        <v>0.5</v>
+      </c>
       <c r="H9" s="19">
         <f ca="1">IF(AND(Liste_de_tâches[[#This Row],[État ]]="Terminée",Liste_de_tâches[[#This Row],[% achevé]]=1),1,IF(ISBLANK(Liste_de_tâches[[#This Row],[Échéance ]]),2,IF(AND(Liste_de_tâches[[#This Row],[État ]]&lt;&gt;"Terminée",TODAY()&gt;Liste_de_tâches[[#This Row],[Échéance ]]),3,2)))</f>
         <v>2</v>
       </c>
-      <c r="I9" s="14"/>
+      <c r="I9" s="14" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="10" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="C10" s="14"/>
-      <c r="D10" s="14"/>
-      <c r="E10" s="15"/>
-      <c r="F10" s="15"/>
-      <c r="G10" s="18"/>
+      <c r="C10" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="E10" s="15">
+        <v>42468</v>
+      </c>
+      <c r="F10" s="15">
+        <v>42472</v>
+      </c>
+      <c r="G10" s="16">
+        <v>0.5</v>
+      </c>
       <c r="H10" s="19">
         <f ca="1">IF(AND(Liste_de_tâches[[#This Row],[État ]]="Terminée",Liste_de_tâches[[#This Row],[% achevé]]=1),1,IF(ISBLANK(Liste_de_tâches[[#This Row],[Échéance ]]),2,IF(AND(Liste_de_tâches[[#This Row],[État ]]&lt;&gt;"Terminée",TODAY()&gt;Liste_de_tâches[[#This Row],[Échéance ]]),3,2)))</f>
         <v>2</v>
       </c>
-      <c r="I10" s="14"/>
+      <c r="I10" s="14" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="11" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="C11" s="14"/>
-      <c r="D11" s="14"/>
-      <c r="E11" s="15"/>
-      <c r="F11" s="15"/>
-      <c r="G11" s="18"/>
+      <c r="C11" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E11" s="15">
+        <v>42468</v>
+      </c>
+      <c r="F11" s="15">
+        <v>42472</v>
+      </c>
+      <c r="G11" s="16">
+        <v>0.75</v>
+      </c>
       <c r="H11" s="19">
         <f ca="1">IF(AND(Liste_de_tâches[[#This Row],[État ]]="Terminée",Liste_de_tâches[[#This Row],[% achevé]]=1),1,IF(ISBLANK(Liste_de_tâches[[#This Row],[Échéance ]]),2,IF(AND(Liste_de_tâches[[#This Row],[État ]]&lt;&gt;"Terminée",TODAY()&gt;Liste_de_tâches[[#This Row],[Échéance ]]),3,2)))</f>
         <v>2</v>
       </c>
-      <c r="I11" s="14"/>
+      <c r="I11" s="14" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="12" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="C12" s="14"/>
-      <c r="D12" s="14"/>
-      <c r="E12" s="15"/>
-      <c r="F12" s="15"/>
-      <c r="G12" s="18"/>
+      <c r="C12" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="D12" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E12" s="15">
+        <v>42468</v>
+      </c>
+      <c r="F12" s="15">
+        <v>42472</v>
+      </c>
+      <c r="G12" s="16">
+        <v>1</v>
+      </c>
       <c r="H12" s="19">
         <f ca="1">IF(AND(Liste_de_tâches[[#This Row],[État ]]="Terminée",Liste_de_tâches[[#This Row],[% achevé]]=1),1,IF(ISBLANK(Liste_de_tâches[[#This Row],[Échéance ]]),2,IF(AND(Liste_de_tâches[[#This Row],[État ]]&lt;&gt;"Terminée",TODAY()&gt;Liste_de_tâches[[#This Row],[Échéance ]]),3,2)))</f>
-        <v>2</v>
-      </c>
-      <c r="I12" s="14"/>
+        <v>1</v>
+      </c>
+      <c r="I12" s="14" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="13" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="C13" s="14"/>
-      <c r="D13" s="14"/>
-      <c r="E13" s="15"/>
-      <c r="F13" s="15"/>
-      <c r="G13" s="18"/>
+      <c r="C13" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="D13" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E13" s="15">
+        <v>42468</v>
+      </c>
+      <c r="F13" s="15">
+        <v>42472</v>
+      </c>
+      <c r="G13" s="16">
+        <v>0.75</v>
+      </c>
       <c r="H13" s="19">
         <f ca="1">IF(AND(Liste_de_tâches[[#This Row],[État ]]="Terminée",Liste_de_tâches[[#This Row],[% achevé]]=1),1,IF(ISBLANK(Liste_de_tâches[[#This Row],[Échéance ]]),2,IF(AND(Liste_de_tâches[[#This Row],[État ]]&lt;&gt;"Terminée",TODAY()&gt;Liste_de_tâches[[#This Row],[Échéance ]]),3,2)))</f>
         <v>2</v>
       </c>
-      <c r="I13" s="14"/>
+      <c r="I13" s="14" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="14" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="14" t="s">
@@ -1438,14 +1501,22 @@
       <c r="D14" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="E14" s="15"/>
-      <c r="F14" s="15"/>
-      <c r="G14" s="18"/>
+      <c r="E14" s="15">
+        <v>42468</v>
+      </c>
+      <c r="F14" s="15">
+        <v>42472</v>
+      </c>
+      <c r="G14" s="16">
+        <v>1</v>
+      </c>
       <c r="H14" s="19">
         <f ca="1">IF(AND(Liste_de_tâches[[#This Row],[État ]]="Terminée",Liste_de_tâches[[#This Row],[% achevé]]=1),1,IF(ISBLANK(Liste_de_tâches[[#This Row],[Échéance ]]),2,IF(AND(Liste_de_tâches[[#This Row],[État ]]&lt;&gt;"Terminée",TODAY()&gt;Liste_de_tâches[[#This Row],[Échéance ]]),3,2)))</f>
-        <v>2</v>
-      </c>
-      <c r="I14" s="14"/>
+        <v>1</v>
+      </c>
+      <c r="I14" s="14" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="15" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="14" t="s">
@@ -1598,10 +1669,10 @@
     <dataValidation type="list" allowBlank="1" sqref="G5:G23">
       <formula1>"0%,25%,50%,75%,100%"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" errorTitle="Whoops" sqref="C5:C8 C14:C15">
+    <dataValidation type="list" allowBlank="1" errorTitle="Whoops" sqref="C5:C15">
       <formula1>"Basse, Normale, Élevée"</formula1>
     </dataValidation>
-    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Whoops" error="For this template to work correctly you need to select a choice from the drop down list. But you can still use what you entered by clicking Yes." sqref="D5:D8 D14:D15">
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Whoops" error="For this template to work correctly you need to select a choice from the drop down list. But you can still use what you entered by clicking Yes." sqref="D5:D15">
       <formula1>"Non commencée,En cours de réalisation, Différé, Terminée"</formula1>
     </dataValidation>
     <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Whoops" error="For this template to work correctly, your Due Date needs to be greater than or equal to the Start Date." sqref="F5:F23">

</xml_diff>

<commit_message>
Modified a lot of file
Charte of Projet --> just correct fault, modified date and verified with all team
Spécifications History Treasures --> Add my part of works
Planning --> change date of Itération 0
Reportin indiv --> for specification to allow correctly
Add 2 pictures (we put this picture in charte)
</commit_message>
<xml_diff>
--- a/Reporting_indiv.xlsx
+++ b/Reporting_indiv.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="40">
   <si>
     <r>
       <rPr>
@@ -165,6 +165,42 @@
   </si>
   <si>
     <t>Julie</t>
+  </si>
+  <si>
+    <t>Spécification</t>
+  </si>
+  <si>
+    <t>Equipe</t>
+  </si>
+  <si>
+    <t>Mission &amp; Objectifs</t>
+  </si>
+  <si>
+    <t>Glossaire</t>
+  </si>
+  <si>
+    <t>Normale</t>
+  </si>
+  <si>
+    <t>Acteurs</t>
+  </si>
+  <si>
+    <t>Cas d'utilisation</t>
+  </si>
+  <si>
+    <t>Yacine et Estéban</t>
+  </si>
+  <si>
+    <t>Carte de navigation</t>
+  </si>
+  <si>
+    <t>Détails des cas d'utilisation</t>
+  </si>
+  <si>
+    <t>Contrainte de conception et d'implémentation</t>
+  </si>
+  <si>
+    <t>Documentation</t>
   </si>
 </sst>
 </file>
@@ -229,7 +265,7 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -263,6 +299,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE2AC76"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -318,7 +360,7 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -390,6 +432,21 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -791,6 +848,7 @@
   </tableStyles>
   <colors>
     <mruColors>
+      <color rgb="FFE2AC76"/>
       <color rgb="FFFF8181"/>
     </mruColors>
   </colors>
@@ -924,7 +982,7 @@
                 <a:schemeClr val="bg1"/>
               </a:solidFill>
             </a:rPr>
-            <a:t>2012</a:t>
+            <a:t>2016</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -935,8 +993,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Liste_de_tâches" displayName="Liste_de_tâches" ref="B4:I23" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
-  <autoFilter ref="B4:I23"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Liste_de_tâches" displayName="Liste_de_tâches" ref="B4:I28" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
+  <autoFilter ref="B4:I28"/>
   <tableColumns count="8">
     <tableColumn id="1" name="Tâche" dataDxfId="7"/>
     <tableColumn id="3" name="Priorité " dataDxfId="6"/>
@@ -1199,10 +1257,10 @@
     <tabColor theme="3" tint="0.39997558519241921"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:I23"/>
+  <dimension ref="B1:I28"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="26.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1373,7 +1431,7 @@
         <v>42472</v>
       </c>
       <c r="G9" s="16">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
       <c r="H9" s="19">
         <f ca="1">IF(AND(Liste_de_tâches[[#This Row],[État ]]="Terminée",Liste_de_tâches[[#This Row],[% achevé]]=1),1,IF(ISBLANK(Liste_de_tâches[[#This Row],[Échéance ]]),2,IF(AND(Liste_de_tâches[[#This Row],[État ]]&lt;&gt;"Terminée",TODAY()&gt;Liste_de_tâches[[#This Row],[Échéance ]]),3,2)))</f>
@@ -1400,7 +1458,7 @@
         <v>42472</v>
       </c>
       <c r="G10" s="16">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
       <c r="H10" s="19">
         <f ca="1">IF(AND(Liste_de_tâches[[#This Row],[État ]]="Terminée",Liste_de_tâches[[#This Row],[% achevé]]=1),1,IF(ISBLANK(Liste_de_tâches[[#This Row],[Échéance ]]),2,IF(AND(Liste_de_tâches[[#This Row],[État ]]&lt;&gt;"Terminée",TODAY()&gt;Liste_de_tâches[[#This Row],[Échéance ]]),3,2)))</f>
@@ -1427,11 +1485,11 @@
         <v>42472</v>
       </c>
       <c r="G11" s="16">
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="H11" s="19">
         <f ca="1">IF(AND(Liste_de_tâches[[#This Row],[État ]]="Terminée",Liste_de_tâches[[#This Row],[% achevé]]=1),1,IF(ISBLANK(Liste_de_tâches[[#This Row],[Échéance ]]),2,IF(AND(Liste_de_tâches[[#This Row],[État ]]&lt;&gt;"Terminée",TODAY()&gt;Liste_de_tâches[[#This Row],[Échéance ]]),3,2)))</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I11" s="14" t="s">
         <v>27</v>
@@ -1481,11 +1539,11 @@
         <v>42472</v>
       </c>
       <c r="G13" s="16">
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="H13" s="19">
         <f ca="1">IF(AND(Liste_de_tâches[[#This Row],[État ]]="Terminée",Liste_de_tâches[[#This Row],[% achevé]]=1),1,IF(ISBLANK(Liste_de_tâches[[#This Row],[Échéance ]]),2,IF(AND(Liste_de_tâches[[#This Row],[État ]]&lt;&gt;"Terminée",TODAY()&gt;Liste_de_tâches[[#This Row],[Échéance ]]),3,2)))</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I13" s="14" t="s">
         <v>27</v>
@@ -1546,112 +1604,295 @@
       </c>
     </row>
     <row r="16" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="14"/>
-      <c r="C16" s="14"/>
-      <c r="D16" s="14"/>
-      <c r="E16" s="15"/>
-      <c r="F16" s="15"/>
-      <c r="G16" s="18"/>
-      <c r="H16" s="19">
+      <c r="B16" s="24" t="s">
+        <v>28</v>
+      </c>
+      <c r="C16" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="D16" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="E16" s="25">
+        <v>42472</v>
+      </c>
+      <c r="F16" s="25">
+        <v>42475</v>
+      </c>
+      <c r="G16" s="26">
+        <v>1</v>
+      </c>
+      <c r="H16" s="27">
         <f ca="1">IF(AND(Liste_de_tâches[[#This Row],[État ]]="Terminée",Liste_de_tâches[[#This Row],[% achevé]]=1),1,IF(ISBLANK(Liste_de_tâches[[#This Row],[Échéance ]]),2,IF(AND(Liste_de_tâches[[#This Row],[État ]]&lt;&gt;"Terminée",TODAY()&gt;Liste_de_tâches[[#This Row],[Échéance ]]),3,2)))</f>
         <v>2</v>
       </c>
-      <c r="I16" s="14"/>
+      <c r="I16" s="24" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="17" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="14"/>
-      <c r="C17" s="14"/>
-      <c r="D17" s="14"/>
-      <c r="E17" s="15"/>
-      <c r="F17" s="15"/>
-      <c r="G17" s="18"/>
+      <c r="B17" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="C17" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="D17" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E17" s="15">
+        <v>42472</v>
+      </c>
+      <c r="F17" s="15">
+        <v>42472</v>
+      </c>
+      <c r="G17" s="16">
+        <v>1</v>
+      </c>
       <c r="H17" s="19">
         <f ca="1">IF(AND(Liste_de_tâches[[#This Row],[État ]]="Terminée",Liste_de_tâches[[#This Row],[% achevé]]=1),1,IF(ISBLANK(Liste_de_tâches[[#This Row],[Échéance ]]),2,IF(AND(Liste_de_tâches[[#This Row],[État ]]&lt;&gt;"Terminée",TODAY()&gt;Liste_de_tâches[[#This Row],[Échéance ]]),3,2)))</f>
+        <v>1</v>
+      </c>
+      <c r="I17" s="14" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="18" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="C18" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="D18" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E18" s="15">
+        <v>42472</v>
+      </c>
+      <c r="F18" s="15">
+        <v>42472</v>
+      </c>
+      <c r="G18" s="16">
+        <v>1</v>
+      </c>
+      <c r="H18" s="19">
+        <f ca="1">IF(AND(Liste_de_tâches[[#This Row],[État ]]="Terminée",Liste_de_tâches[[#This Row],[% achevé]]=1),1,IF(ISBLANK(Liste_de_tâches[[#This Row],[Échéance ]]),2,IF(AND(Liste_de_tâches[[#This Row],[État ]]&lt;&gt;"Terminée",TODAY()&gt;Liste_de_tâches[[#This Row],[Échéance ]]),3,2)))</f>
+        <v>1</v>
+      </c>
+      <c r="I18" s="14" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="19" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="C19" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="D19" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E19" s="15">
+        <v>42472</v>
+      </c>
+      <c r="F19" s="15">
+        <v>42472</v>
+      </c>
+      <c r="G19" s="16">
+        <v>1</v>
+      </c>
+      <c r="H19" s="19">
+        <f ca="1">IF(AND(Liste_de_tâches[[#This Row],[État ]]="Terminée",Liste_de_tâches[[#This Row],[% achevé]]=1),1,IF(ISBLANK(Liste_de_tâches[[#This Row],[Échéance ]]),2,IF(AND(Liste_de_tâches[[#This Row],[État ]]&lt;&gt;"Terminée",TODAY()&gt;Liste_de_tâches[[#This Row],[Échéance ]]),3,2)))</f>
+        <v>1</v>
+      </c>
+      <c r="I19" s="14" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="C20" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="D20" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E20" s="15">
+        <v>42472</v>
+      </c>
+      <c r="F20" s="15">
+        <v>42472</v>
+      </c>
+      <c r="G20" s="16">
+        <v>1</v>
+      </c>
+      <c r="H20" s="19">
+        <f ca="1">IF(AND(Liste_de_tâches[[#This Row],[État ]]="Terminée",Liste_de_tâches[[#This Row],[% achevé]]=1),1,IF(ISBLANK(Liste_de_tâches[[#This Row],[Échéance ]]),2,IF(AND(Liste_de_tâches[[#This Row],[État ]]&lt;&gt;"Terminée",TODAY()&gt;Liste_de_tâches[[#This Row],[Échéance ]]),3,2)))</f>
+        <v>1</v>
+      </c>
+      <c r="I20" s="14" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="21" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="C21" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="D21" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E21" s="15">
+        <v>42472</v>
+      </c>
+      <c r="F21" s="15"/>
+      <c r="G21" s="16">
+        <v>1</v>
+      </c>
+      <c r="H21" s="19">
+        <f ca="1">IF(AND(Liste_de_tâches[[#This Row],[État ]]="Terminée",Liste_de_tâches[[#This Row],[% achevé]]=1),1,IF(ISBLANK(Liste_de_tâches[[#This Row],[Échéance ]]),2,IF(AND(Liste_de_tâches[[#This Row],[État ]]&lt;&gt;"Terminée",TODAY()&gt;Liste_de_tâches[[#This Row],[Échéance ]]),3,2)))</f>
+        <v>1</v>
+      </c>
+      <c r="I21" s="14" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="22" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="C22" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="D22" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E22" s="15">
+        <v>42472</v>
+      </c>
+      <c r="F22" s="15"/>
+      <c r="G22" s="16">
+        <v>1</v>
+      </c>
+      <c r="H22" s="19">
+        <f ca="1">IF(AND(Liste_de_tâches[[#This Row],[État ]]="Terminée",Liste_de_tâches[[#This Row],[% achevé]]=1),1,IF(ISBLANK(Liste_de_tâches[[#This Row],[Échéance ]]),2,IF(AND(Liste_de_tâches[[#This Row],[État ]]&lt;&gt;"Terminée",TODAY()&gt;Liste_de_tâches[[#This Row],[Échéance ]]),3,2)))</f>
+        <v>1</v>
+      </c>
+      <c r="I22" s="14" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="23" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="C23" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="D23" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E23" s="21">
+        <v>42472</v>
+      </c>
+      <c r="F23" s="21"/>
+      <c r="G23" s="28">
+        <v>1</v>
+      </c>
+      <c r="H23" s="23">
+        <f ca="1">IF(AND(Liste_de_tâches[[#This Row],[État ]]="Terminée",Liste_de_tâches[[#This Row],[% achevé]]=1),1,IF(ISBLANK(Liste_de_tâches[[#This Row],[Échéance ]]),2,IF(AND(Liste_de_tâches[[#This Row],[État ]]&lt;&gt;"Terminée",TODAY()&gt;Liste_de_tâches[[#This Row],[Échéance ]]),3,2)))</f>
+        <v>1</v>
+      </c>
+      <c r="I23" s="20" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="24" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="C24" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="D24" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E24" s="15">
+        <v>42472</v>
+      </c>
+      <c r="F24" s="15"/>
+      <c r="G24" s="16">
+        <v>1</v>
+      </c>
+      <c r="H24" s="19">
+        <f ca="1">IF(AND(Liste_de_tâches[[#This Row],[État ]]="Terminée",Liste_de_tâches[[#This Row],[% achevé]]=1),1,IF(ISBLANK(Liste_de_tâches[[#This Row],[Échéance ]]),2,IF(AND(Liste_de_tâches[[#This Row],[État ]]&lt;&gt;"Terminée",TODAY()&gt;Liste_de_tâches[[#This Row],[Échéance ]]),3,2)))</f>
+        <v>1</v>
+      </c>
+      <c r="I24" s="14" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="25" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="14"/>
+      <c r="C25" s="14"/>
+      <c r="D25" s="14"/>
+      <c r="E25" s="15"/>
+      <c r="F25" s="15"/>
+      <c r="G25" s="18"/>
+      <c r="H25" s="19">
+        <f ca="1">IF(AND(Liste_de_tâches[[#This Row],[État ]]="Terminée",Liste_de_tâches[[#This Row],[% achevé]]=1),1,IF(ISBLANK(Liste_de_tâches[[#This Row],[Échéance ]]),2,IF(AND(Liste_de_tâches[[#This Row],[État ]]&lt;&gt;"Terminée",TODAY()&gt;Liste_de_tâches[[#This Row],[Échéance ]]),3,2)))</f>
         <v>2</v>
       </c>
-      <c r="I17" s="14"/>
-    </row>
-    <row r="18" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="14"/>
-      <c r="C18" s="14"/>
-      <c r="D18" s="14"/>
-      <c r="E18" s="15"/>
-      <c r="F18" s="15"/>
-      <c r="G18" s="18"/>
-      <c r="H18" s="19">
+      <c r="I25" s="14"/>
+    </row>
+    <row r="26" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="14"/>
+      <c r="C26" s="14"/>
+      <c r="D26" s="14"/>
+      <c r="E26" s="15"/>
+      <c r="F26" s="15"/>
+      <c r="G26" s="18"/>
+      <c r="H26" s="19">
         <f ca="1">IF(AND(Liste_de_tâches[[#This Row],[État ]]="Terminée",Liste_de_tâches[[#This Row],[% achevé]]=1),1,IF(ISBLANK(Liste_de_tâches[[#This Row],[Échéance ]]),2,IF(AND(Liste_de_tâches[[#This Row],[État ]]&lt;&gt;"Terminée",TODAY()&gt;Liste_de_tâches[[#This Row],[Échéance ]]),3,2)))</f>
         <v>2</v>
       </c>
-      <c r="I18" s="14"/>
-    </row>
-    <row r="19" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="14"/>
-      <c r="C19" s="14"/>
-      <c r="D19" s="14"/>
-      <c r="E19" s="15"/>
-      <c r="F19" s="15"/>
-      <c r="G19" s="18"/>
-      <c r="H19" s="19">
+      <c r="I26" s="14"/>
+    </row>
+    <row r="27" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="14"/>
+      <c r="C27" s="14"/>
+      <c r="D27" s="14"/>
+      <c r="E27" s="15"/>
+      <c r="F27" s="15"/>
+      <c r="G27" s="18"/>
+      <c r="H27" s="19">
         <f ca="1">IF(AND(Liste_de_tâches[[#This Row],[État ]]="Terminée",Liste_de_tâches[[#This Row],[% achevé]]=1),1,IF(ISBLANK(Liste_de_tâches[[#This Row],[Échéance ]]),2,IF(AND(Liste_de_tâches[[#This Row],[État ]]&lt;&gt;"Terminée",TODAY()&gt;Liste_de_tâches[[#This Row],[Échéance ]]),3,2)))</f>
         <v>2</v>
       </c>
-      <c r="I19" s="14"/>
-    </row>
-    <row r="20" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="14"/>
-      <c r="C20" s="14"/>
-      <c r="D20" s="14"/>
-      <c r="E20" s="15"/>
-      <c r="F20" s="15"/>
-      <c r="G20" s="18"/>
-      <c r="H20" s="19">
+      <c r="I27" s="14"/>
+    </row>
+    <row r="28" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B28" s="20"/>
+      <c r="C28" s="20"/>
+      <c r="D28" s="20"/>
+      <c r="E28" s="21"/>
+      <c r="F28" s="21"/>
+      <c r="G28" s="22"/>
+      <c r="H28" s="23">
         <f ca="1">IF(AND(Liste_de_tâches[[#This Row],[État ]]="Terminée",Liste_de_tâches[[#This Row],[% achevé]]=1),1,IF(ISBLANK(Liste_de_tâches[[#This Row],[Échéance ]]),2,IF(AND(Liste_de_tâches[[#This Row],[État ]]&lt;&gt;"Terminée",TODAY()&gt;Liste_de_tâches[[#This Row],[Échéance ]]),3,2)))</f>
         <v>2</v>
       </c>
-      <c r="I20" s="14"/>
-    </row>
-    <row r="21" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="14"/>
-      <c r="C21" s="14"/>
-      <c r="D21" s="14"/>
-      <c r="E21" s="15"/>
-      <c r="F21" s="15"/>
-      <c r="G21" s="18"/>
-      <c r="H21" s="19">
-        <f ca="1">IF(AND(Liste_de_tâches[[#This Row],[État ]]="Terminée",Liste_de_tâches[[#This Row],[% achevé]]=1),1,IF(ISBLANK(Liste_de_tâches[[#This Row],[Échéance ]]),2,IF(AND(Liste_de_tâches[[#This Row],[État ]]&lt;&gt;"Terminée",TODAY()&gt;Liste_de_tâches[[#This Row],[Échéance ]]),3,2)))</f>
-        <v>2</v>
-      </c>
-      <c r="I21" s="14"/>
-    </row>
-    <row r="22" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="14"/>
-      <c r="C22" s="14"/>
-      <c r="D22" s="14"/>
-      <c r="E22" s="15"/>
-      <c r="F22" s="15"/>
-      <c r="G22" s="18"/>
-      <c r="H22" s="19">
-        <f ca="1">IF(AND(Liste_de_tâches[[#This Row],[État ]]="Terminée",Liste_de_tâches[[#This Row],[% achevé]]=1),1,IF(ISBLANK(Liste_de_tâches[[#This Row],[Échéance ]]),2,IF(AND(Liste_de_tâches[[#This Row],[État ]]&lt;&gt;"Terminée",TODAY()&gt;Liste_de_tâches[[#This Row],[Échéance ]]),3,2)))</f>
-        <v>2</v>
-      </c>
-      <c r="I22" s="14"/>
-    </row>
-    <row r="23" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="20"/>
-      <c r="C23" s="20"/>
-      <c r="D23" s="20"/>
-      <c r="E23" s="21"/>
-      <c r="F23" s="21"/>
-      <c r="G23" s="22"/>
-      <c r="H23" s="23">
-        <f ca="1">IF(AND(Liste_de_tâches[[#This Row],[État ]]="Terminée",Liste_de_tâches[[#This Row],[% achevé]]=1),1,IF(ISBLANK(Liste_de_tâches[[#This Row],[Échéance ]]),2,IF(AND(Liste_de_tâches[[#This Row],[État ]]&lt;&gt;"Terminée",TODAY()&gt;Liste_de_tâches[[#This Row],[Échéance ]]),3,2)))</f>
-        <v>2</v>
-      </c>
-      <c r="I23" s="20"/>
+      <c r="I28" s="20"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
-  <conditionalFormatting sqref="G5:G23">
+  <conditionalFormatting sqref="G5:G28">
     <cfRule type="dataBar" priority="59">
       <dataBar>
         <cfvo type="min"/>
@@ -1666,16 +1907,16 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" sqref="G5:G23">
+    <dataValidation type="list" allowBlank="1" sqref="G5:G28">
       <formula1>"0%,25%,50%,75%,100%"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" errorTitle="Whoops" sqref="C5:C15">
+    <dataValidation type="list" allowBlank="1" errorTitle="Whoops" sqref="C5:C24">
       <formula1>"Basse, Normale, Élevée"</formula1>
     </dataValidation>
-    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Whoops" error="For this template to work correctly you need to select a choice from the drop down list. But you can still use what you entered by clicking Yes." sqref="D5:D15">
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Whoops" error="For this template to work correctly you need to select a choice from the drop down list. But you can still use what you entered by clicking Yes." sqref="D5:D24">
       <formula1>"Non commencée,En cours de réalisation, Différé, Terminée"</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Whoops" error="For this template to work correctly, your Due Date needs to be greater than or equal to the Start Date." sqref="F5:F23">
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Whoops" error="For this template to work correctly, your Due Date needs to be greater than or equal to the Start Date." sqref="F5:F28">
       <formula1>F5&gt;=E5</formula1>
     </dataValidation>
   </dataValidations>
@@ -1702,7 +1943,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>G5:G23</xm:sqref>
+          <xm:sqref>G5:G28</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="iconSet" priority="60" id="{61976558-4184-4BD1-B78A-DCBE6FDA3BC9}">
@@ -1721,7 +1962,7 @@
               <x14:cfIcon iconSet="3Flags" iconId="0"/>
             </x14:iconSet>
           </x14:cfRule>
-          <xm:sqref>H5:H23</xm:sqref>
+          <xm:sqref>H5:H28</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>

</xml_diff>

<commit_message>
Changed dead line --> 26/04/2016
Because dead line for itération 0 is in 26/04/2016
</commit_message>
<xml_diff>
--- a/Reporting_indiv.xlsx
+++ b/Reporting_indiv.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="39">
   <si>
     <r>
       <rPr>
@@ -123,9 +123,6 @@
   </si>
   <si>
     <t>Charte de projet</t>
-  </si>
-  <si>
-    <t>En cours de réalisation</t>
   </si>
   <si>
     <t xml:space="preserve">A terminer </t>
@@ -360,7 +357,7 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -447,6 +444,18 @@
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -1259,8 +1268,8 @@
   </sheetPr>
   <dimension ref="B1:I28"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="26.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1320,7 +1329,7 @@
         <v>42467</v>
       </c>
       <c r="F5" s="6">
-        <v>42471</v>
+        <v>42486</v>
       </c>
       <c r="G5" s="7">
         <v>1</v>
@@ -1341,28 +1350,28 @@
         <v>7</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="E6" s="6">
         <v>42468</v>
       </c>
       <c r="F6" s="6">
-        <v>42472</v>
+        <v>42486</v>
       </c>
       <c r="G6" s="7">
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="H6" s="8">
         <f ca="1">IF(AND(Liste_de_tâches[[#This Row],[État ]]="Terminée",Liste_de_tâches[[#This Row],[% achevé]]=1),1,IF(ISBLANK(Liste_de_tâches[[#This Row],[Échéance ]]),2,IF(AND(Liste_de_tâches[[#This Row],[État ]]&lt;&gt;"Terminée",TODAY()&gt;Liste_de_tâches[[#This Row],[Échéance ]]),3,2)))</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I6" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C7" s="10" t="s">
         <v>9</v>
@@ -1374,7 +1383,7 @@
         <v>42468</v>
       </c>
       <c r="F7" s="11">
-        <v>42472</v>
+        <v>42486</v>
       </c>
       <c r="G7" s="12">
         <v>1</v>
@@ -1384,12 +1393,12 @@
         <v>1</v>
       </c>
       <c r="I7" s="9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="17" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C8" s="14" t="s">
         <v>9</v>
@@ -1401,7 +1410,7 @@
         <v>42468</v>
       </c>
       <c r="F8" s="15">
-        <v>42472</v>
+        <v>42486</v>
       </c>
       <c r="G8" s="16">
         <v>1</v>
@@ -1411,66 +1420,66 @@
         <v>1</v>
       </c>
       <c r="I8" s="14" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="14" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C9" s="14" t="s">
         <v>9</v>
       </c>
       <c r="D9" s="14" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="E9" s="15">
         <v>42468</v>
       </c>
       <c r="F9" s="15">
-        <v>42472</v>
+        <v>42486</v>
       </c>
       <c r="G9" s="16">
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="H9" s="19">
         <f ca="1">IF(AND(Liste_de_tâches[[#This Row],[État ]]="Terminée",Liste_de_tâches[[#This Row],[% achevé]]=1),1,IF(ISBLANK(Liste_de_tâches[[#This Row],[Échéance ]]),2,IF(AND(Liste_de_tâches[[#This Row],[État ]]&lt;&gt;"Terminée",TODAY()&gt;Liste_de_tâches[[#This Row],[Échéance ]]),3,2)))</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I9" s="14" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="14" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C10" s="14" t="s">
         <v>9</v>
       </c>
       <c r="D10" s="14" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="E10" s="15">
         <v>42468</v>
       </c>
       <c r="F10" s="15">
-        <v>42472</v>
+        <v>42486</v>
       </c>
       <c r="G10" s="16">
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="H10" s="19">
         <f ca="1">IF(AND(Liste_de_tâches[[#This Row],[État ]]="Terminée",Liste_de_tâches[[#This Row],[% achevé]]=1),1,IF(ISBLANK(Liste_de_tâches[[#This Row],[Échéance ]]),2,IF(AND(Liste_de_tâches[[#This Row],[État ]]&lt;&gt;"Terminée",TODAY()&gt;Liste_de_tâches[[#This Row],[Échéance ]]),3,2)))</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I10" s="14" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C11" s="14" t="s">
         <v>9</v>
@@ -1482,7 +1491,7 @@
         <v>42468</v>
       </c>
       <c r="F11" s="15">
-        <v>42472</v>
+        <v>42486</v>
       </c>
       <c r="G11" s="16">
         <v>1</v>
@@ -1492,12 +1501,12 @@
         <v>1</v>
       </c>
       <c r="I11" s="14" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="14" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C12" s="14" t="s">
         <v>9</v>
@@ -1509,7 +1518,7 @@
         <v>42468</v>
       </c>
       <c r="F12" s="15">
-        <v>42472</v>
+        <v>42486</v>
       </c>
       <c r="G12" s="16">
         <v>1</v>
@@ -1519,12 +1528,12 @@
         <v>1</v>
       </c>
       <c r="I12" s="14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="13" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="14" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C13" s="14" t="s">
         <v>9</v>
@@ -1536,7 +1545,7 @@
         <v>42468</v>
       </c>
       <c r="F13" s="15">
-        <v>42472</v>
+        <v>42486</v>
       </c>
       <c r="G13" s="16">
         <v>1</v>
@@ -1546,12 +1555,12 @@
         <v>1</v>
       </c>
       <c r="I13" s="14" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="14" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="14" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C14" s="14" t="s">
         <v>9</v>
@@ -1563,7 +1572,7 @@
         <v>42468</v>
       </c>
       <c r="F14" s="15">
-        <v>42472</v>
+        <v>42486</v>
       </c>
       <c r="G14" s="16">
         <v>1</v>
@@ -1573,12 +1582,12 @@
         <v>1</v>
       </c>
       <c r="I14" s="14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="15" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C15" s="14" t="s">
         <v>9</v>
@@ -1590,7 +1599,7 @@
         <v>42471</v>
       </c>
       <c r="F15" s="15">
-        <v>42471</v>
+        <v>42486</v>
       </c>
       <c r="G15" s="16">
         <v>1</v>
@@ -1600,39 +1609,39 @@
         <v>1</v>
       </c>
       <c r="I15" s="14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="16" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="24" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C16" s="24" t="s">
         <v>9</v>
       </c>
       <c r="D16" s="24" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="E16" s="25">
         <v>42472</v>
       </c>
       <c r="F16" s="25">
-        <v>42475</v>
+        <v>42486</v>
       </c>
       <c r="G16" s="26">
         <v>1</v>
       </c>
       <c r="H16" s="27">
         <f ca="1">IF(AND(Liste_de_tâches[[#This Row],[État ]]="Terminée",Liste_de_tâches[[#This Row],[% achevé]]=1),1,IF(ISBLANK(Liste_de_tâches[[#This Row],[Échéance ]]),2,IF(AND(Liste_de_tâches[[#This Row],[État ]]&lt;&gt;"Terminée",TODAY()&gt;Liste_de_tâches[[#This Row],[Échéance ]]),3,2)))</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I16" s="24" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="17" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="14" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C17" s="14" t="s">
         <v>9</v>
@@ -1644,7 +1653,7 @@
         <v>42472</v>
       </c>
       <c r="F17" s="15">
-        <v>42472</v>
+        <v>42486</v>
       </c>
       <c r="G17" s="16">
         <v>1</v>
@@ -1654,15 +1663,15 @@
         <v>1</v>
       </c>
       <c r="I17" s="14" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="18" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="C18" s="14" t="s">
         <v>31</v>
-      </c>
-      <c r="C18" s="14" t="s">
-        <v>32</v>
       </c>
       <c r="D18" s="14" t="s">
         <v>10</v>
@@ -1671,7 +1680,7 @@
         <v>42472</v>
       </c>
       <c r="F18" s="15">
-        <v>42472</v>
+        <v>42486</v>
       </c>
       <c r="G18" s="16">
         <v>1</v>
@@ -1681,12 +1690,12 @@
         <v>1</v>
       </c>
       <c r="I18" s="14" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="19" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="14" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C19" s="14" t="s">
         <v>9</v>
@@ -1698,7 +1707,7 @@
         <v>42472</v>
       </c>
       <c r="F19" s="15">
-        <v>42472</v>
+        <v>42486</v>
       </c>
       <c r="G19" s="16">
         <v>1</v>
@@ -1708,12 +1717,12 @@
         <v>1</v>
       </c>
       <c r="I19" s="14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="20" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="14" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C20" s="14" t="s">
         <v>9</v>
@@ -1725,7 +1734,7 @@
         <v>42472</v>
       </c>
       <c r="F20" s="15">
-        <v>42472</v>
+        <v>42486</v>
       </c>
       <c r="G20" s="16">
         <v>1</v>
@@ -1735,12 +1744,12 @@
         <v>1</v>
       </c>
       <c r="I20" s="14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="21" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C21" s="14" t="s">
         <v>9</v>
@@ -1751,7 +1760,9 @@
       <c r="E21" s="15">
         <v>42472</v>
       </c>
-      <c r="F21" s="15"/>
+      <c r="F21" s="15">
+        <v>42486</v>
+      </c>
       <c r="G21" s="16">
         <v>1</v>
       </c>
@@ -1760,12 +1771,12 @@
         <v>1</v>
       </c>
       <c r="I21" s="14" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="22" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="14" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C22" s="14" t="s">
         <v>9</v>
@@ -1776,7 +1787,9 @@
       <c r="E22" s="15">
         <v>42472</v>
       </c>
-      <c r="F22" s="15"/>
+      <c r="F22" s="15">
+        <v>42486</v>
+      </c>
       <c r="G22" s="16">
         <v>1</v>
       </c>
@@ -1785,12 +1798,12 @@
         <v>1</v>
       </c>
       <c r="I22" s="14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="23" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="20" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C23" s="14" t="s">
         <v>9</v>
@@ -1801,7 +1814,9 @@
       <c r="E23" s="21">
         <v>42472</v>
       </c>
-      <c r="F23" s="21"/>
+      <c r="F23" s="15">
+        <v>42486</v>
+      </c>
       <c r="G23" s="28">
         <v>1</v>
       </c>
@@ -1810,12 +1825,12 @@
         <v>1</v>
       </c>
       <c r="I23" s="20" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="24" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="14" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C24" s="14" t="s">
         <v>9</v>
@@ -1826,7 +1841,9 @@
       <c r="E24" s="15">
         <v>42472</v>
       </c>
-      <c r="F24" s="15"/>
+      <c r="F24" s="15">
+        <v>42486</v>
+      </c>
       <c r="G24" s="16">
         <v>1</v>
       </c>
@@ -1835,21 +1852,21 @@
         <v>1</v>
       </c>
       <c r="I24" s="14" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="25" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="14"/>
-      <c r="C25" s="14"/>
-      <c r="D25" s="14"/>
-      <c r="E25" s="15"/>
-      <c r="F25" s="15"/>
-      <c r="G25" s="18"/>
-      <c r="H25" s="19">
+      <c r="B25" s="29"/>
+      <c r="C25" s="29"/>
+      <c r="D25" s="29"/>
+      <c r="E25" s="30"/>
+      <c r="F25" s="30"/>
+      <c r="G25" s="31"/>
+      <c r="H25" s="32">
         <f ca="1">IF(AND(Liste_de_tâches[[#This Row],[État ]]="Terminée",Liste_de_tâches[[#This Row],[% achevé]]=1),1,IF(ISBLANK(Liste_de_tâches[[#This Row],[Échéance ]]),2,IF(AND(Liste_de_tâches[[#This Row],[État ]]&lt;&gt;"Terminée",TODAY()&gt;Liste_de_tâches[[#This Row],[Échéance ]]),3,2)))</f>
         <v>2</v>
       </c>
-      <c r="I25" s="14"/>
+      <c r="I25" s="29"/>
     </row>
     <row r="26" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="14"/>

</xml_diff>